<commit_message>
Pretty much finalized the first version of the experiment. Added quite a few more fprintf statements with trial information.
</commit_message>
<xml_diff>
--- a/po-cond01-test.xlsx
+++ b/po-cond01-test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="2380" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cond01.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>condN</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>blank</t>
+  </si>
+  <si>
+    <t>cont1_lo</t>
+  </si>
+  <si>
+    <t>cont7_lo</t>
   </si>
 </sst>
 </file>
@@ -127,8 +133,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -152,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -162,6 +176,10 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -171,6 +189,10 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -566,13 +588,13 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="E2">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -602,33 +624,33 @@
         <v>10</v>
       </c>
       <c r="O2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P2">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>20</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>0.01</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="E3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
         <v>500</v>
@@ -652,10 +674,10 @@
         <v>10</v>
       </c>
       <c r="O3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P3">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -663,16 +685,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="D4">
-        <v>1E-3</v>
+        <v>0.02</v>
       </c>
       <c r="E4">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -702,10 +724,110 @@
         <v>10</v>
       </c>
       <c r="O4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P4">
-        <v>34</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>0.01</v>
+      </c>
+      <c r="D5">
+        <v>0.02</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>500</v>
+      </c>
+      <c r="I5">
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+      <c r="K5">
+        <v>0.2</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>250</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+      <c r="E6">
+        <v>1E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>500</v>
+      </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
+      <c r="J6">
+        <v>0.5</v>
+      </c>
+      <c r="K6">
+        <v>0.2</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>250</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented the best PEST adaptive staircase. Dealt with the termination errors and, hopefully, the lag. Messed with the priors but found the defaults to be working well, at least for my threshold.
</commit_message>
<xml_diff>
--- a/po-cond01-test.xlsx
+++ b/po-cond01-test.xlsx
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="D2">
         <v>0.02</v>
@@ -688,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
         <v>0.02</v>

</xml_diff>

<commit_message>
Added the equiluminance module and changed the pop-out salience levels.
</commit_message>
<xml_diff>
--- a/po-cond01-test.xlsx
+++ b/po-cond01-test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>condN</t>
   </si>
@@ -54,15 +54,6 @@
     <t>odtT</t>
   </si>
   <si>
-    <t>vcSt</t>
-  </si>
-  <si>
-    <t>vcUp</t>
-  </si>
-  <si>
-    <t>vcDn</t>
-  </si>
-  <si>
     <t>postStimBlankT</t>
   </si>
   <si>
@@ -85,6 +76,9 @@
   </si>
   <si>
     <t>cont7_lo</t>
+  </si>
+  <si>
+    <t>odtLoc</t>
   </si>
 </sst>
 </file>
@@ -133,8 +127,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -166,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -180,6 +176,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -193,6 +190,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -522,15 +520,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,295 +536,259 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="N1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>0.8</v>
+      <c r="C2" t="s">
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>0.02</v>
+        <v>0.3</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
+        <v>500</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
       </c>
       <c r="G2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H2">
-        <v>500</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
-        <v>1000</v>
+        <v>12</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>250</v>
       </c>
       <c r="K2">
-        <v>0.2</v>
+        <v>10</v>
       </c>
       <c r="L2">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>250</v>
+        <v>1.5</v>
       </c>
       <c r="N2">
-        <v>10</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-      <c r="P2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>0.01</v>
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>0.02</v>
+        <v>0.3</v>
       </c>
       <c r="E3">
-        <v>0.01</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+        <v>500</v>
+      </c>
+      <c r="F3">
+        <v>1000</v>
       </c>
       <c r="G3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
-        <v>500</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>12</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>250</v>
       </c>
       <c r="K3">
-        <v>0.2</v>
+        <v>10</v>
       </c>
       <c r="L3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M3">
-        <v>250</v>
+        <v>1.5</v>
       </c>
       <c r="N3">
-        <v>10</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
-      <c r="P3">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
         <v>0.8</v>
       </c>
-      <c r="D4">
-        <v>0.02</v>
-      </c>
       <c r="E4">
-        <v>0.01</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
+        <v>500</v>
+      </c>
+      <c r="F4">
+        <v>1000</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
-        <v>500</v>
+        <v>0.2</v>
       </c>
       <c r="I4">
-        <v>1000</v>
+        <v>12</v>
       </c>
       <c r="J4">
-        <v>0.5</v>
+        <v>250</v>
       </c>
       <c r="K4">
-        <v>0.2</v>
+        <v>10</v>
       </c>
       <c r="L4">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>250</v>
+        <v>1.5</v>
       </c>
       <c r="N4">
-        <v>10</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5">
-        <v>0.01</v>
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>0.02</v>
+        <v>0.8</v>
       </c>
       <c r="E5">
-        <v>0.01</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
+        <v>500</v>
+      </c>
+      <c r="F5">
+        <v>1000</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H5">
-        <v>500</v>
+        <v>0.2</v>
       </c>
       <c r="I5">
-        <v>1000</v>
+        <v>12</v>
       </c>
       <c r="J5">
-        <v>0.5</v>
+        <v>250</v>
       </c>
       <c r="K5">
-        <v>0.2</v>
+        <v>10</v>
       </c>
       <c r="L5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M5">
-        <v>250</v>
+        <v>1.5</v>
       </c>
       <c r="N5">
-        <v>10</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="D6">
-        <v>1E-3</v>
-      </c>
       <c r="E6">
-        <v>1E-3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
+        <v>500</v>
+      </c>
+      <c r="F6">
+        <v>1000</v>
       </c>
       <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>250</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>500</v>
-      </c>
-      <c r="I6">
-        <v>1000</v>
-      </c>
-      <c r="J6">
-        <v>0.5</v>
-      </c>
-      <c r="K6">
-        <v>0.2</v>
-      </c>
-      <c r="L6">
-        <v>12</v>
-      </c>
       <c r="M6">
-        <v>250</v>
+        <v>1.5</v>
       </c>
       <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
-      <c r="P6">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A slew of changes: wrote the preliminary threshold program and rewrote the main program to N-up-N-down staircase. A bunch of fixes.
</commit_message>
<xml_diff>
--- a/po-cond01-test.xlsx
+++ b/po-cond01-test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cond01.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>condN</t>
   </si>
@@ -79,6 +79,21 @@
   </si>
   <si>
     <t>odtLoc</t>
+  </si>
+  <si>
+    <t>maskOnOff</t>
+  </si>
+  <si>
+    <t>nRevs</t>
+  </si>
+  <si>
+    <t>stairUp</t>
+  </si>
+  <si>
+    <t>stairDn</t>
+  </si>
+  <si>
+    <t>dnDivUp</t>
   </si>
 </sst>
 </file>
@@ -195,6 +210,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -520,15 +540,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,8 +591,23 @@
       <c r="N1" t="s">
         <v>10</v>
       </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -615,8 +650,23 @@
       <c r="N2">
         <v>17</v>
       </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -659,8 +709,23 @@
       <c r="N3">
         <v>17</v>
       </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -703,8 +768,23 @@
       <c r="N4">
         <v>17</v>
       </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -747,8 +827,23 @@
       <c r="N5">
         <v>17</v>
       </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -790,6 +885,21 @@
       </c>
       <c r="N6">
         <v>17</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the final staircase. Randomized non-primed locations. Provided feedback during the trial as to the current answer (very helpfulConverted to linear ramp-up (kept the gaussian ramp just in case). Also included a no-ramp option in both the code and the conditions file. Included a table of ODT accuracy as a function of location and tilt.
</commit_message>
<xml_diff>
--- a/po-cond01-test.xlsx
+++ b/po-cond01-test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cond01.csv" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
     <t>stairDn</t>
   </si>
   <si>
-    <t>dnDivUp</t>
+    <t>stepUpMulti</t>
   </si>
 </sst>
 </file>
@@ -542,13 +542,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:R1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +607,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -660,13 +660,13 @@
         <v>1</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -701,7 +701,7 @@
         <v>10</v>
       </c>
       <c r="L3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>1.5</v>
@@ -719,13 +719,13 @@
         <v>1</v>
       </c>
       <c r="R3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4">
         <v>3</v>
       </c>
@@ -778,13 +778,13 @@
         <v>1</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -819,7 +819,7 @@
         <v>10</v>
       </c>
       <c r="L5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>1.5</v>
@@ -837,13 +837,13 @@
         <v>1</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -896,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="R6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S6">
         <v>4</v>

</xml_diff>

<commit_message>
A bunch of changes that are hard to track at this point. Committing everything just in case, sieving through it later.
</commit_message>
<xml_diff>
--- a/po-cond01-test.xlsx
+++ b/po-cond01-test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>condN</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>stepUpMulti</t>
+  </si>
+  <si>
+    <t>stimRamp</t>
+  </si>
+  <si>
+    <t>rampLin</t>
+  </si>
+  <si>
+    <t>logStep</t>
+  </si>
+  <si>
+    <t>maskRamp</t>
   </si>
 </sst>
 </file>
@@ -540,15 +552,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="F2" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,37 +589,49 @@
         <v>14</v>
       </c>
       <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,7 +648,7 @@
         <v>500</v>
       </c>
       <c r="F2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G2">
         <v>0.5</v>
@@ -636,37 +660,49 @@
         <v>12</v>
       </c>
       <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>250</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>0</v>
       </c>
-      <c r="M2">
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>1.5</v>
       </c>
-      <c r="N2">
+      <c r="R2">
         <v>17</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>4</v>
-      </c>
       <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>4</v>
+      </c>
+      <c r="W2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>2</v>
       </c>
@@ -683,7 +719,7 @@
         <v>500</v>
       </c>
       <c r="F3">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G3">
         <v>0.5</v>
@@ -695,37 +731,49 @@
         <v>12</v>
       </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>250</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>10</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>1.5</v>
       </c>
-      <c r="N3">
+      <c r="R3">
         <v>17</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>4</v>
-      </c>
       <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="W3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>3</v>
       </c>
@@ -742,7 +790,7 @@
         <v>500</v>
       </c>
       <c r="F4">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G4">
         <v>0.5</v>
@@ -754,37 +802,49 @@
         <v>12</v>
       </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>250</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>10</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="M4">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>1.5</v>
       </c>
-      <c r="N4">
+      <c r="R4">
         <v>17</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4">
-        <v>4</v>
-      </c>
       <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
+        <v>4</v>
+      </c>
+      <c r="W4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>4</v>
       </c>
@@ -801,7 +861,7 @@
         <v>500</v>
       </c>
       <c r="F5">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G5">
         <v>0.5</v>
@@ -813,37 +873,49 @@
         <v>12</v>
       </c>
       <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>250</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>10</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
         <v>1.5</v>
       </c>
-      <c r="N5">
+      <c r="R5">
         <v>17</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>4</v>
-      </c>
       <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>4</v>
+      </c>
+      <c r="W5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:23">
       <c r="A6">
         <v>5</v>
       </c>
@@ -860,7 +932,7 @@
         <v>500</v>
       </c>
       <c r="F6">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G6">
         <v>0.5</v>
@@ -872,33 +944,45 @@
         <v>12</v>
       </c>
       <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>250</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>10</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>1.5</v>
       </c>
-      <c r="N6">
+      <c r="R6">
         <v>17</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>4</v>
-      </c>
       <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
+        <v>4</v>
+      </c>
+      <c r="W6">
         <v>4</v>
       </c>
     </row>

</xml_diff>